<commit_message>
new test cases of fixed intervals, updated readme
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,43 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Digital World/SecureFileTransfer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{611B573A-80B1-3844-93BE-EAEC722464AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CC3C24-E40F-D84C-BD89-9CBC6635F571}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="440" windowWidth="28040" windowHeight="16280" xr2:uid="{31AE6C5F-F3FA-CA4A-88E8-5716046C62C4}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="27460" windowHeight="16260" xr2:uid="{31AE6C5F-F3FA-CA4A-88E8-5716046C62C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$E$2:$E$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v2.12" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v2.13" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v2.14" hidden="1">Sheet1!$D$2:$D$8</definedName>
-    <definedName name="_xlchart.v2.15" hidden="1">Sheet1!$E$2:$E$8</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$F$2:$F$10</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$G$2:$G$10</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$F$2:$F$10</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$G$2:$G$10</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Size</t>
   </si>
@@ -65,6 +53,36 @@
   </si>
   <si>
     <t xml:space="preserve">In conclusion: Symmetric key is faster :D </t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>rr0.txt</t>
+  </si>
+  <si>
+    <t>rr1.txt</t>
+  </si>
+  <si>
+    <t>rr2.txt</t>
+  </si>
+  <si>
+    <t>rr3.txt</t>
+  </si>
+  <si>
+    <t>rr4.txt</t>
+  </si>
+  <si>
+    <t>rr6.txt</t>
+  </si>
+  <si>
+    <t>rr7.txt</t>
+  </si>
+  <si>
+    <t>File size (kb)</t>
+  </si>
+  <si>
+    <t>rr5.txt</t>
   </si>
 </sst>
 </file>
@@ -200,7 +218,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -221,7 +239,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -257,7 +275,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -278,7 +296,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$8</c:f>
+              <c:f>Sheet1!$G$2:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -505,7 +523,442 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput with</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> increasing size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CP1 TP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0173478998589562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.40495080043980208</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8108259940231073E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.6521906625842805E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4910121682245203E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8661686949357441E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5271-C141-9B25-E87F45B5E46E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CP2 TP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.241661035260931</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21773709015942824</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0057512160402588E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0888979492855824E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1905991538664885E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4662447997763713E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5271-C141-9B25-E87F45B5E46E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="760558287"/>
+        <c:axId val="760559983"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="760558287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760559983"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="760559983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="760558287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1048,17 +1501,533 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1081,6 +2050,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3F05444-8E27-1341-BF65-D6C571FDB3C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1386,147 +2391,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB75137-0CA8-454D-9D51-75E4CC50E989}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>126</v>
+      </c>
+      <c r="C2">
         <v>721.29966100000001</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>880.33767399999999</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>709</v>
       </c>
-      <c r="D2">
-        <f>A2/C2</f>
+      <c r="F2">
+        <f t="shared" ref="F2:F7" si="0">C2/E2</f>
         <v>1.0173478998589562</v>
       </c>
-      <c r="E2">
-        <f>B2/C2</f>
+      <c r="G2">
+        <f>D2/E2</f>
         <v>1.241661035260931</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>252</v>
+      </c>
+      <c r="C3">
         <v>736.60550599999999</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>396.06376699999998</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>1819</v>
       </c>
-      <c r="D3">
-        <f>A3/C3</f>
+      <c r="F3">
+        <f t="shared" si="0"/>
         <v>0.40495080043980208</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">B3/C3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="1">D3/E3</f>
         <v>0.21773709015942824</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>505</v>
+      </c>
+      <c r="C4">
         <v>6114.6982799999996</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>718.74913900000001</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>897791</v>
       </c>
-      <c r="D4">
-        <f>A4/C4</f>
+      <c r="F4">
+        <f t="shared" si="0"/>
         <v>6.8108259940231073E-3</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>8.0057512160402588E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5">
+        <v>10286.931734</v>
+      </c>
+      <c r="D5">
+        <v>818.53785800000003</v>
+      </c>
+      <c r="E5">
+        <v>1344312</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="0"/>
-        <v>8.0057512160402588E-4</v>
+        <v>7.6521906625842805E-3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>6.0888979492855824E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>10286.931734</v>
-      </c>
-      <c r="B5">
-        <v>818.53785800000003</v>
-      </c>
-      <c r="C5">
-        <v>1344312</v>
-      </c>
-      <c r="D5">
-        <f>A5/C5</f>
-        <v>7.6521906625842805E-3</v>
-      </c>
-      <c r="E5">
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2000</v>
+      </c>
+      <c r="C6">
+        <v>15188.596487999999</v>
+      </c>
+      <c r="D6">
+        <v>1052.4334269999999</v>
+      </c>
+      <c r="E6">
+        <v>2027576</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>6.0888979492855824E-4</v>
+        <v>7.4910121682245203E-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5.1905991538664885E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>15188.596487999999</v>
-      </c>
-      <c r="B6">
-        <v>1052.4334269999999</v>
-      </c>
-      <c r="C6">
-        <v>2027576</v>
-      </c>
-      <c r="D6">
-        <f>A6/C6</f>
-        <v>7.4910121682245203E-3</v>
-      </c>
-      <c r="E6">
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>4000</v>
+      </c>
+      <c r="C7">
+        <v>16039.865255000001</v>
+      </c>
+      <c r="D7">
+        <v>910.709744</v>
+      </c>
+      <c r="E7">
+        <v>2039095</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>5.1905991538664885E-4</v>
+        <v>7.8661686949357441E-3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>4.4662447997763713E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>16039.865255000001</v>
-      </c>
-      <c r="B7">
-        <v>910.709744</v>
-      </c>
-      <c r="C7">
-        <v>2039095</v>
-      </c>
-      <c r="D7">
-        <f>A7/C7</f>
-        <v>7.8661686949357441E-3</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>4.4662447997763713E-4</v>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>8000</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated excel, removed comments, deleted unnecessary files and updated readme
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Digital World/SecureFileTransfer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CC3C24-E40F-D84C-BD89-9CBC6635F571}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB4124A-CB20-E94C-9E4E-2DAA06FE841F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27460" windowHeight="16260" xr2:uid="{31AE6C5F-F3FA-CA4A-88E8-5716046C62C4}"/>
   </bookViews>
@@ -36,24 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>CP1 Time</t>
-  </si>
-  <si>
-    <t>CP2 Time</t>
-  </si>
-  <si>
-    <t>CP2 TP</t>
-  </si>
-  <si>
-    <t>CP1 TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In conclusion: Symmetric key is faster :D </t>
-  </si>
   <si>
     <t>File name</t>
   </si>
@@ -83,6 +65,24 @@
   </si>
   <si>
     <t>rr5.txt</t>
+  </si>
+  <si>
+    <t>CP1 Time (ms)</t>
+  </si>
+  <si>
+    <t>File size (bytes)</t>
+  </si>
+  <si>
+    <t>CP2 Time (ms)</t>
+  </si>
+  <si>
+    <t>CP2 Throughput</t>
+  </si>
+  <si>
+    <t>CP1 Throughput</t>
+  </si>
+  <si>
+    <t>In conclusion: Symmetric key is faster :D Throughput increases exponentially as file size increases</t>
   </si>
 </sst>
 </file>
@@ -118,8 +118,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,7 +225,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CP1 TP</c:v>
+                  <c:v>CP1 Throughput</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -244,22 +247,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.0173478998589562</c:v>
+                  <c:v>127.07777232296426</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40495080043980208</c:v>
+                  <c:v>159.41692012304682</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8108259940231073E-3</c:v>
+                  <c:v>162.28575353588042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6521906625842805E-3</c:v>
+                  <c:v>130.64371119789968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4910121682245203E-3</c:v>
+                  <c:v>198.49253797875716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.8661686949357441E-3</c:v>
+                  <c:v>116.04537475082762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111.02010799436073</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -275,11 +281,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CP2 Time</c:v>
+                  <c:v>CP2 Time (ms)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -301,22 +307,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.241661035260931</c:v>
+                  <c:v>129.30251253293173</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21773709015942824</c:v>
+                  <c:v>284.10537682620725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0057512160402588E-4</c:v>
+                  <c:v>535.2372812134131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0888979492855824E-4</c:v>
+                  <c:v>870.86722999538279</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1905991538664885E-4</c:v>
+                  <c:v>1436.2335003790313</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4662447997763713E-4</c:v>
+                  <c:v>2007.2166917818756</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2760.1901300377544</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,7 +567,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput with</a:t>
+              <a:t>Throughput (bytes/time) with</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -612,7 +621,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CP1 TP</c:v>
+                  <c:v>CP1 Throughput</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -636,22 +645,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.0173478998589562</c:v>
+                  <c:v>127.07777232296426</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40495080043980208</c:v>
+                  <c:v>159.41692012304682</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8108259940231073E-3</c:v>
+                  <c:v>162.28575353588042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.6521906625842805E-3</c:v>
+                  <c:v>130.64371119789968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4910121682245203E-3</c:v>
+                  <c:v>198.49253797875716</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.8661686949357441E-3</c:v>
+                  <c:v>116.04537475082762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>111.02010799436073</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>116.94157380347788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,7 +687,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CP2 TP</c:v>
+                  <c:v>CP2 Throughput</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -696,22 +711,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.241661035260931</c:v>
+                  <c:v>129.30251253293173</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.21773709015942824</c:v>
+                  <c:v>284.10537682620725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0057512160402588E-4</c:v>
+                  <c:v>535.2372812134131</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0888979492855824E-4</c:v>
+                  <c:v>870.86722999538279</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.1905991538664885E-4</c:v>
+                  <c:v>1436.2335003790313</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4662447997763713E-4</c:v>
+                  <c:v>2007.2166917818756</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2760.1901300377544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3783.682553493858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2021,16 +2042,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>927100</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2058,15 +2079,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
+      <xdr:colOff>673100</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:colOff>317500</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2391,210 +2412,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB75137-0CA8-454D-9D51-75E4CC50E989}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="35" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>126</v>
       </c>
       <c r="C2">
-        <v>721.29966100000001</v>
+        <v>126150</v>
       </c>
       <c r="D2">
-        <v>880.33767399999999</v>
+        <v>992.69917699999996</v>
       </c>
       <c r="E2">
-        <v>709</v>
+        <v>975.61909300000002</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F7" si="0">C2/E2</f>
-        <v>1.0173478998589562</v>
+        <f>C2/D2</f>
+        <v>127.07777232296426</v>
       </c>
       <c r="G2">
-        <f>D2/E2</f>
-        <v>1.241661035260931</v>
+        <f>C2/E2</f>
+        <v>129.30251253293173</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>252</v>
       </c>
       <c r="C3">
-        <v>736.60550599999999</v>
+        <v>252399</v>
       </c>
       <c r="D3">
-        <v>396.06376699999998</v>
+        <v>1583.263557</v>
       </c>
       <c r="E3">
-        <v>1819</v>
+        <v>888.39923699999997</v>
       </c>
       <c r="F3">
-        <f t="shared" si="0"/>
-        <v>0.40495080043980208</v>
+        <f t="shared" ref="F3:F9" si="0">C3/D3</f>
+        <v>159.41692012304682</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G7" si="1">D3/E3</f>
-        <v>0.21773709015942824</v>
+        <f t="shared" ref="G3:G9" si="1">C3/E3</f>
+        <v>284.10537682620725</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>505</v>
       </c>
       <c r="C4">
-        <v>6114.6982799999996</v>
+        <v>504900</v>
       </c>
       <c r="D4">
-        <v>718.74913900000001</v>
+        <v>3111.178825</v>
       </c>
       <c r="E4">
-        <v>897791</v>
+        <v>943.31993999999997</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>6.8108259940231073E-3</v>
+        <v>162.28575353588042</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>8.0057512160402588E-4</v>
+        <v>535.2372812134131</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1000</v>
       </c>
       <c r="C5">
-        <v>10286.931734</v>
+        <v>1009899</v>
       </c>
       <c r="D5">
-        <v>818.53785800000003</v>
+        <v>7730.1769119999999</v>
       </c>
       <c r="E5">
-        <v>1344312</v>
+        <v>1159.6474929999999</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>7.6521906625842805E-3</v>
+        <v>130.64371119789968</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>6.0888979492855824E-4</v>
+        <v>870.86722999538279</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2000</v>
       </c>
       <c r="C6">
-        <v>15188.596487999999</v>
+        <v>2019901</v>
       </c>
       <c r="D6">
-        <v>1052.4334269999999</v>
+        <v>10176.206222000001</v>
       </c>
       <c r="E6">
-        <v>2027576</v>
+        <v>1406.38761</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>7.4910121682245203E-3</v>
+        <v>198.49253797875716</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>5.1905991538664885E-4</v>
+        <v>1436.2335003790313</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>4000</v>
       </c>
       <c r="C7">
-        <v>16039.865255000001</v>
+        <v>4039800</v>
       </c>
       <c r="D7">
-        <v>910.709744</v>
+        <v>34812.244853999997</v>
       </c>
       <c r="E7">
-        <v>2039095</v>
+        <v>2012.6377070000001</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>7.8661686949357441E-3</v>
+        <v>116.04537475082762</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>4.4662447997763713E-4</v>
+        <v>2007.2166917818756</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>8000</v>
+      </c>
+      <c r="C8">
+        <v>8079600</v>
+      </c>
+      <c r="D8">
+        <v>72776.005590000001</v>
+      </c>
+      <c r="E8">
+        <v>2927.1896569999999</v>
+      </c>
+      <c r="F8">
+        <f>C8/D8</f>
+        <v>111.02010799436073</v>
+      </c>
+      <c r="G8">
+        <f>C8/E8</f>
+        <v>2760.1901300377544</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>16000</v>
       </c>
+      <c r="C9">
+        <v>16159200</v>
+      </c>
+      <c r="D9">
+        <v>138181.82425999999</v>
+      </c>
+      <c r="E9">
+        <v>4270.7599730000002</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>116.94157380347788</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>3783.682553493858</v>
+      </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="C10" t="s">
-        <v>5</v>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>